<commit_message>
correcao analisse de eventos
</commit_message>
<xml_diff>
--- a/artefatos/Análise de Eventos.xlsx
+++ b/artefatos/Análise de Eventos.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabriel.alves\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080F02E0-2466-43F3-83A5-97EB148F86D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11145"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
   <si>
     <t>Capacidade</t>
   </si>
@@ -58,9 +52,6 @@
   </si>
   <si>
     <t xml:space="preserve">Não Evento* </t>
-  </si>
-  <si>
-    <t>Cliente verifica data disponível</t>
   </si>
   <si>
     <t>Cliente agenda data</t>
@@ -140,12 +131,18 @@
   </si>
   <si>
     <t>x(14)</t>
+  </si>
+  <si>
+    <t>FA</t>
+  </si>
+  <si>
+    <t>Cliente solicita data disponível</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -304,6 +301,42 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -313,15 +346,6 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -338,33 +362,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -639,18 +636,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,34 +666,34 @@
   <sheetData>
     <row r="1" spans="2:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21" t="s">
+      <c r="C2" s="15"/>
+      <c r="D2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="25"/>
-      <c r="H2" s="24" t="s">
+      <c r="G2" s="19"/>
+      <c r="H2" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="20" t="s">
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="14" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="23"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="17"/>
       <c r="F3" s="3" t="s">
         <v>3</v>
       </c>
@@ -712,24 +709,24 @@
       <c r="J3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="20"/>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="26" t="s">
-        <v>29</v>
+      <c r="K3" s="14"/>
+    </row>
+    <row r="4" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="8" t="s">
+        <v>28</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
@@ -737,16 +734,16 @@
       <c r="K4" s="7"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="27"/>
+      <c r="B5" s="9"/>
       <c r="C5" s="12"/>
       <c r="D5" s="2">
         <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="4"/>
@@ -755,16 +752,16 @@
       <c r="K5" s="7"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="27"/>
+      <c r="B6" s="9"/>
       <c r="C6" s="12"/>
       <c r="D6" s="2">
         <v>3</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="4"/>
@@ -773,53 +770,55 @@
       <c r="K6" s="7"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="27"/>
-      <c r="C7" s="12"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="12" t="s">
+        <v>37</v>
+      </c>
       <c r="D7" s="2">
         <v>4</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="7"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="28"/>
+    <row r="8" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="10"/>
       <c r="C8" s="13"/>
       <c r="D8" s="2">
         <v>5</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="7"/>
     </row>
     <row r="9" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="14" t="s">
-        <v>30</v>
+      <c r="B9" s="23" t="s">
+        <v>29</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" s="2">
         <v>6</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
@@ -827,17 +826,17 @@
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="15"/>
+      <c r="B10" s="24"/>
       <c r="C10" s="12"/>
       <c r="D10" s="2">
         <v>7</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
@@ -845,17 +844,17 @@
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="15"/>
+      <c r="B11" s="24"/>
       <c r="C11" s="12"/>
       <c r="D11" s="2">
         <v>8</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
@@ -863,17 +862,17 @@
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="16"/>
+      <c r="B12" s="25"/>
       <c r="C12" s="13"/>
       <c r="D12" s="2">
         <v>9</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
@@ -881,21 +880,21 @@
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="17" t="s">
-        <v>31</v>
+      <c r="B13" s="26" t="s">
+        <v>30</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" s="2">
         <v>10</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
@@ -903,17 +902,17 @@
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="18"/>
+      <c r="B14" s="27"/>
       <c r="C14" s="12"/>
       <c r="D14" s="2">
         <v>11</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
@@ -921,57 +920,57 @@
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="18"/>
+      <c r="B15" s="27"/>
       <c r="C15" s="12"/>
       <c r="D15" s="2">
         <v>12</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="7"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="19"/>
+      <c r="B16" s="28"/>
       <c r="C16" s="13"/>
       <c r="D16" s="2">
         <v>13</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="7"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="8" t="s">
-        <v>32</v>
+      <c r="B17" s="20" t="s">
+        <v>31</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D17" s="2">
         <v>14</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
@@ -979,79 +978,80 @@
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="9"/>
+      <c r="B18" s="21"/>
       <c r="C18" s="12"/>
       <c r="D18" s="2">
         <v>15</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="7"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="9"/>
+      <c r="B19" s="21"/>
       <c r="C19" s="12"/>
       <c r="D19" s="2">
         <v>16</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="7"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="10"/>
+      <c r="B20" s="22"/>
       <c r="C20" s="13"/>
       <c r="D20" s="2">
         <v>17</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="15">
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="C17:C20"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="C9:C12"/>
+    <mergeCell ref="C13:C16"/>
     <mergeCell ref="B4:B8"/>
-    <mergeCell ref="C4:C8"/>
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="B2:C3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="F2:G2"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="C17:C20"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="C9:C12"/>
-    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="C7:C8"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>